<commit_message>
data and table upload
</commit_message>
<xml_diff>
--- a/Table descLAST.xlsx
+++ b/Table descLAST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altanbagana.n\source\repos\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADFBFC62-F508-4EE1-B921-537A360088DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD62CE26-B9DB-497A-BEF1-DF5865C22D5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -909,7 +909,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -946,6 +946,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -959,7 +965,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -974,6 +980,7 @@
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1358,8 +1365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G73" sqref="G73"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1387,7 +1394,7 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="14" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1456,7 +1463,7 @@
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="14" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="4" t="s">

</xml_diff>

<commit_message>
all messed up combo and database mismatch
</commit_message>
<xml_diff>
--- a/Table descLAST.xlsx
+++ b/Table descLAST.xlsx
@@ -1,23 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altanbagana.n\source\repos\pages\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD62CE26-B9DB-497A-BEF1-DF5865C22D5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="23256" windowHeight="13176" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
-    <sheet name="State" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="State" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="293">
   <si>
     <t>Boards</t>
   </si>
@@ -861,16 +856,65 @@
   </si>
   <si>
     <t>4020.000000</t>
+  </si>
+  <si>
+    <t>төрөл 0-арилжааны данс, 1-клирингийн данс, 2-төлбөр тооцооны данс, 3-барьцааны данс, 4-зээлийн данс</t>
+  </si>
+  <si>
+    <t>+1 - орлого/-1 - зарлага</t>
+  </si>
+  <si>
+    <t>AssetBalances</t>
+  </si>
+  <si>
+    <t>1-долоо хоногийн өдрүүд</t>
+  </si>
+  <si>
+    <t>1-Даваа, 2-Мягмар ... Өдрүүдийг ";" тэмдэгтээр тусгаарласан байна</t>
+  </si>
+  <si>
+    <t>төлөв /State sheet-ээс харна уу/</t>
+  </si>
+  <si>
+    <t>тулгалт хийх алгоритм 0-тулгалт хийхгүй, 1-FIFO, 2-Equilbrium</t>
+  </si>
+  <si>
+    <t>зах зээлийн төрөл 0-margin, 2-DvP</t>
+  </si>
+  <si>
+    <t>зөвшөөрөх захиалгын төрөл 1-Зах зээлийн
+2-Нөхцөлт
+3-Кросс
+4-Тохиролцсон
+5-Зах зээл үүсгэгч</t>
+  </si>
+  <si>
+    <t>Үнэт цаасны төрөл 1-үнэт цаас, 2-бонд</t>
+  </si>
+  <si>
+    <t>гэрээний төрөл 1-спот, 2-форвард, 3-фьючерс, 4-опцион</t>
+  </si>
+  <si>
+    <t>авах талын дэнчинг тооцох төрөл 0-үнийн дүнгээс хувиар, 1-тогтмол дүнгээр</t>
+  </si>
+  <si>
+    <t>зарах талын дэнчинг тооцох төрөл 0-үнийн дүнгээс хувиар, 1-тогтмол дүнгээр</t>
+  </si>
+  <si>
+    <t>Төрөл 1-арилжаа, 2-ОТС, 3-Тохиролцоо, 4-Репо, 5-Зээл, 6-Барьцаа, 7-М2М</t>
+  </si>
+  <si>
+    <t>Төрөл 1-арилжаа, 2-ОТС, 3-Тохиролцоо</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]m/d/yyyy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -908,8 +952,22 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -952,6 +1010,30 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -965,7 +1047,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -981,6 +1063,24 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1355,30 +1455,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S204"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="19" width="20.7109375" customWidth="1"/>
-    <col min="20" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="4" max="19" width="20.6640625" customWidth="1"/>
+    <col min="20" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1393,7 +1493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>3</v>
       </c>
@@ -1416,7 +1516,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1439,11 +1539,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -1459,7 +1559,7 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -1518,7 +1618,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1577,7 +1677,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>55</v>
       </c>
@@ -1586,7 +1686,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>3</v>
       </c>
@@ -1627,7 +1727,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1662,7 +1762,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C12" s="8"/>
       <c r="D12" s="9"/>
       <c r="E12" s="8"/>
@@ -1671,7 +1771,7 @@
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>175</v>
       </c>
@@ -1691,7 +1791,7 @@
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
@@ -1738,7 +1838,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1782,7 +1882,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C16" s="8"/>
       <c r="D16" s="9"/>
       <c r="E16" s="8"/>
@@ -1791,14 +1891,14 @@
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>3</v>
       </c>
@@ -1827,7 +1927,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -1856,7 +1956,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>195</v>
       </c>
@@ -1876,7 +1976,7 @@
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>3</v>
       </c>
@@ -1923,7 +2023,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -1967,7 +2067,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>225</v>
       </c>
@@ -1986,7 +2086,7 @@
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>3</v>
       </c>
@@ -2027,7 +2127,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>3</v>
       </c>
@@ -2069,7 +2169,7 @@
       </c>
       <c r="N27" s="9"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>149</v>
       </c>
@@ -2083,7 +2183,7 @@
       <c r="G29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>3</v>
       </c>
@@ -2109,7 +2209,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>157</v>
       </c>
@@ -2135,7 +2235,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>164</v>
       </c>
@@ -2149,7 +2249,7 @@
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>3</v>
       </c>
@@ -2184,7 +2284,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="12" t="s">
         <v>3</v>
       </c>
@@ -2219,7 +2319,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>134</v>
       </c>
@@ -2232,7 +2332,7 @@
       <c r="G37" s="10"/>
       <c r="H37" s="10"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>3</v>
       </c>
@@ -2264,7 +2364,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>3</v>
       </c>
@@ -2296,7 +2396,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>219</v>
       </c>
@@ -2307,7 +2407,7 @@
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>3</v>
       </c>
@@ -2327,7 +2427,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>3</v>
       </c>
@@ -2347,7 +2447,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>73</v>
       </c>
@@ -2356,7 +2456,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>3</v>
       </c>
@@ -2397,7 +2497,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>3</v>
       </c>
@@ -2432,7 +2532,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>147</v>
       </c>
@@ -2441,7 +2541,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>3</v>
       </c>
@@ -2458,7 +2558,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>3</v>
       </c>
@@ -2475,7 +2575,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>209</v>
       </c>
@@ -2484,7 +2584,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>3</v>
       </c>
@@ -2495,7 +2595,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>49</v>
       </c>
@@ -2506,7 +2606,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
         <v>213</v>
       </c>
@@ -2515,7 +2615,7 @@
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>3</v>
       </c>
@@ -2538,7 +2638,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>3</v>
       </c>
@@ -2561,7 +2661,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
         <v>46</v>
       </c>
@@ -2570,7 +2670,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>3</v>
       </c>
@@ -2587,7 +2687,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>3</v>
       </c>
@@ -2604,7 +2704,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="10" t="s">
         <v>83</v>
       </c>
@@ -2613,7 +2713,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
         <v>3</v>
       </c>
@@ -2648,7 +2748,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>3</v>
       </c>
@@ -2683,7 +2783,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="10" t="s">
         <v>100</v>
       </c>
@@ -2692,7 +2792,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
         <v>3</v>
       </c>
@@ -2727,7 +2827,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>3</v>
       </c>
@@ -2762,7 +2862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="10" t="s">
         <v>118</v>
       </c>
@@ -2771,7 +2871,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
         <v>3</v>
       </c>
@@ -2797,7 +2897,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>3</v>
       </c>
@@ -2823,7 +2923,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>123</v>
       </c>
@@ -2835,7 +2935,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
         <v>3</v>
       </c>
@@ -2861,7 +2961,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>127</v>
       </c>
@@ -2887,15 +2987,15 @@
         <v>133</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="6"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
         <v>3</v>
       </c>
@@ -2915,7 +3015,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>3</v>
       </c>
@@ -2935,10 +3035,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A105" s="6"/>
     </row>
-    <row r="107" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A107"/>
       <c r="B107"/>
       <c r="C107"/>
@@ -2955,7 +3055,7 @@
       <c r="N107"/>
       <c r="O107"/>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A108" s="9"/>
       <c r="B108" s="9"/>
       <c r="C108" s="9"/>
@@ -2972,100 +3072,100 @@
       <c r="N108" s="9"/>
       <c r="O108" s="9"/>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A111" s="6"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" s="6"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" s="6"/>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" s="6"/>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" s="6"/>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" s="6"/>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" s="6"/>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132" s="6"/>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135" s="6"/>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138" s="6"/>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141" s="6"/>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144" s="6"/>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" s="6"/>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150" s="6"/>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153" s="6"/>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156" s="6"/>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A159" s="6"/>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162" s="6"/>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165" s="6"/>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A168" s="6"/>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A171" s="6"/>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174" s="6"/>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A177" s="6"/>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180" s="6"/>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A183" s="6"/>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186" s="6"/>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189" s="6"/>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192" s="6"/>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195" s="6"/>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198" s="6"/>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A201" s="6"/>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A204" s="6"/>
     </row>
   </sheetData>
@@ -3075,26 +3175,1716 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S204"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.6640625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="28" style="16" customWidth="1"/>
+    <col min="4" max="4" width="28.88671875" style="16" customWidth="1"/>
+    <col min="5" max="19" width="20.6640625" style="16" customWidth="1"/>
+    <col min="20" max="1025" width="8.6640625" style="16" customWidth="1"/>
+    <col min="1026" max="16384" width="9.109375" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C4" s="28" t="s">
+        <v>281</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="N6" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="O6" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="P6" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q6" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="R6" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="S6" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>284</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="M7" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="N7" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="P7" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q7" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="R7" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="S7" s="26" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="K10" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="L10" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="M10" s="17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="J11" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="K11" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C12" s="19"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="J14" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="K14" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="L14" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="M14" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="N14" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="O14" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>287</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="J15" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="K15" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="L15" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="M15" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="N15" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="O15" s="20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C16" s="19"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="I22" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="J22" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="K22" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="L22" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="M22" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="N22" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="O22" s="17" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>288</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="I23" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="K23" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="L23" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="M23" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="N23" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="O23" s="16" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="I26" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="J26" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="K26" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="L26" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="M26" s="17" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D27" s="30" t="s">
+        <v>279</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="G27" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="H27" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="I27" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="J27" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="K27" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="L27" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="M27" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="N27" s="17"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="H30" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>289</v>
+      </c>
+      <c r="E31" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="F34" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="G34" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="H34" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="I34" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="J34" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="K34" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="F35" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="G35" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="H35" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="I35" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="J35" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="K35" s="20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="F38" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H38" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="I38" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="J38" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D39" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="E39" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="F39" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="G39" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="H39" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="I39" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="J39" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="E43" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="F43" s="16" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B45" s="15"/>
+      <c r="C45" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D46" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E46" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F46" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="G46" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="H46" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="I46" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="J46" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="K46" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="L46" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="M46" s="17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D47" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="F47" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G47" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="H47" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="I47" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="J47" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="K47" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D50" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C51" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D51" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="E51" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="C53" s="15" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="C54" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C55" s="16" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" s="15" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="D58" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="E58" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="F58" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="G58" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="D59" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="E59" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="F59" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="G59" s="16" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B61" s="15"/>
+      <c r="C61" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B62" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C62" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D62" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C63" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D63" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E63" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A65" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B65" s="15"/>
+      <c r="C65" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A66" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C66" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="D66" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E66" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="F66" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="G66" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="H66" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="I66" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="J66" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="K66" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A67" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B67" s="26" t="s">
+        <v>292</v>
+      </c>
+      <c r="C67" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D67" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="E67" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="F67" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="G67" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="H67" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="I67" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="J67" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="K67" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A69" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="B69" s="15"/>
+      <c r="C69" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A70" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B70" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C70" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="D70" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="E70" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="F70" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="G70" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="H70" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="I70" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="J70" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="K70" s="17" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A71" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B71" s="26" t="s">
+        <v>291</v>
+      </c>
+      <c r="C71" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="D71" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="E71" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="F71" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="G71" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="H71" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="I71" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="J71" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="K71" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A73" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B73" s="15"/>
+      <c r="C73" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A74" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B74" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="C74" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D74" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="E74" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="F74" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="G74" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="H74" s="17" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A75" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B75" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C75" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="D75" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="E75" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="F75" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G75" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="H75" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A77" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B77" s="15"/>
+      <c r="C77" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="D77" s="16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A78" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B78" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C78" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D78" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E78" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F78" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G78" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H78" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A79" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="B79" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C79" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="D79" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="E79" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="F79" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="G79" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="H79" s="16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A80" s="15"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A84" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A85" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B85" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C85" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D85" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E85" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F85" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A86" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B86" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C86" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D86" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E86" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F86" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A88" s="27" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A89" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B89" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C89" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="D89" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E89" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="F89" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="G89" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H89" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E90" s="16">
+        <v>100</v>
+      </c>
+      <c r="F90" s="16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A105" s="15"/>
+    </row>
+    <row r="107" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="16"/>
+      <c r="B107" s="16"/>
+      <c r="C107" s="16"/>
+      <c r="D107" s="16"/>
+      <c r="E107" s="16"/>
+      <c r="F107" s="16"/>
+      <c r="G107" s="16"/>
+      <c r="H107" s="16"/>
+      <c r="I107" s="16"/>
+      <c r="J107" s="16"/>
+      <c r="K107" s="16"/>
+      <c r="L107" s="16"/>
+      <c r="M107" s="16"/>
+      <c r="N107" s="16"/>
+      <c r="O107" s="16"/>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A108" s="17"/>
+      <c r="B108" s="17"/>
+      <c r="C108" s="17"/>
+      <c r="D108" s="17"/>
+      <c r="E108" s="17"/>
+      <c r="F108" s="17"/>
+      <c r="G108" s="17"/>
+      <c r="H108" s="17"/>
+      <c r="I108" s="17"/>
+      <c r="J108" s="17"/>
+      <c r="K108" s="17"/>
+      <c r="L108" s="17"/>
+      <c r="M108" s="17"/>
+      <c r="N108" s="17"/>
+      <c r="O108" s="17"/>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A111" s="15"/>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114" s="15"/>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117" s="15"/>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120" s="15"/>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123" s="15"/>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A126" s="15"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129" s="15"/>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132" s="15"/>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A135" s="15"/>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A138" s="15"/>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A141" s="15"/>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A144" s="15"/>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A147" s="15"/>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A150" s="15"/>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A153" s="15"/>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A156" s="15"/>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A159" s="15"/>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A162" s="15"/>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A165" s="15"/>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A168" s="15"/>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A171" s="15"/>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A174" s="15"/>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A177" s="15"/>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A180" s="15"/>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A183" s="15"/>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A186" s="15"/>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A189" s="15"/>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A192" s="15"/>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A195" s="15"/>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A198" s="15"/>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A201" s="15"/>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A204" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" customWidth="1"/>
-    <col min="3" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" customWidth="1"/>
+    <col min="3" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>238</v>
       </c>
@@ -3102,7 +4892,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -3110,7 +4900,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>-1</v>
       </c>
@@ -3118,7 +4908,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3126,7 +4916,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>-2</v>
       </c>
@@ -3134,7 +4924,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>99</v>
       </c>
@@ -3148,22 +4938,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -3228,7 +5018,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3293,7 +5083,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
fee insert done change to update
</commit_message>
<xml_diff>
--- a/Table descLAST.xlsx
+++ b/Table descLAST.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altanbagana.n\source\repos\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00B990F-A9E0-41F2-9F72-038B7FB3DD6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA8E89F-F9BE-4D6E-80B2-7723A3406145}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29520" yWindow="9300" windowWidth="28170" windowHeight="12645" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="2340" windowWidth="28170" windowHeight="12645" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="315">
   <si>
     <t>Boards</t>
   </si>
@@ -957,19 +957,10 @@
     <t>memberId</t>
   </si>
   <si>
-    <t>assetAmount</t>
-  </si>
-  <si>
-    <t>pirce</t>
-  </si>
-  <si>
     <t>collateral</t>
   </si>
   <si>
     <t>order</t>
-  </si>
-  <si>
-    <t>orderID</t>
   </si>
   <si>
     <t>from member</t>
@@ -991,7 +982,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]m/d/yyyy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1058,8 +1049,25 @@
       <charset val="1"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1137,8 +1145,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1161,12 +1179,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1205,9 +1240,14 @@
     <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="2" xfId="3"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3301,10 +3341,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:S185"/>
+  <dimension ref="A1:S180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="F118" sqref="F118"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="K110" sqref="K110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4886,7 +4926,7 @@
       </c>
       <c r="B96" s="32"/>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" s="15" t="s">
         <v>299</v>
       </c>
@@ -4894,7 +4934,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" s="33" t="s">
         <v>3</v>
       </c>
@@ -4911,25 +4951,25 @@
         <v>303</v>
       </c>
       <c r="F99" s="16" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="G99" s="35" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" s="15"/>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G103"/>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" s="15" t="s">
         <v>304</v>
       </c>
       <c r="G104"/>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" s="16" t="s">
         <v>3</v>
       </c>
@@ -4950,198 +4990,206 @@
       </c>
       <c r="G105"/>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G106"/>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A107" s="15"/>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A106" s="27"/>
+      <c r="H106"/>
+      <c r="I106"/>
+    </row>
+    <row r="107" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H107"/>
       <c r="I107"/>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J108"/>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A110" s="15"/>
-      <c r="J110"/>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A111" s="27" t="s">
+    <row r="108" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="27" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A112" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B112" s="16" t="s">
+      <c r="B108" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C108" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="D108" s="36" t="s">
+        <v>308</v>
+      </c>
+      <c r="E108" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="F108" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="G108" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="H108" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="I108" s="26" t="s">
         <v>313</v>
       </c>
-      <c r="C112" s="16" t="s">
-        <v>308</v>
-      </c>
-      <c r="D112" s="16" t="s">
+      <c r="J108" s="26" t="s">
+        <v>314</v>
+      </c>
+      <c r="K108" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="L108" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="H109"/>
+      <c r="I109"/>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H110"/>
+      <c r="I110"/>
+    </row>
+    <row r="111" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="15" t="s">
+        <v>310</v>
+      </c>
+      <c r="C111" s="16" t="s">
+        <v>311</v>
+      </c>
+      <c r="H111"/>
+      <c r="I111"/>
+    </row>
+    <row r="112" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B112" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C112" s="17"/>
+      <c r="D112" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="E112" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="F112" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="E112" s="16" t="s">
-        <v>316</v>
-      </c>
-      <c r="F112" s="16" t="s">
-        <v>317</v>
-      </c>
-      <c r="G112" s="16" t="s">
-        <v>309</v>
-      </c>
-      <c r="H112" s="16" t="s">
-        <v>310</v>
-      </c>
-      <c r="I112" s="16" t="s">
+      <c r="G112" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="H112" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="I112" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="J112" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="K112" s="17" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A113" s="15"/>
-    </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A116" s="15" t="s">
+      <c r="L112" s="17"/>
+      <c r="M112" s="17"/>
+    </row>
+    <row r="113" spans="1:11" ht="78.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B113" s="26" t="s">
         <v>312</v>
       </c>
-      <c r="C116" s="16" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A117" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B117" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="C117" s="17"/>
-      <c r="D117" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="E117" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="F117" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="G117" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="H117" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="I117" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="J117" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="K117" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="L117" s="17"/>
-      <c r="M117" s="17"/>
-    </row>
-    <row r="118" spans="1:13" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B118" s="26" t="s">
-        <v>315</v>
-      </c>
-      <c r="D118" s="16" t="s">
+      <c r="D113" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="E118" s="16" t="s">
+      <c r="E113" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="F118" s="16" t="s">
+      <c r="F113" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="G118" s="16" t="s">
+      <c r="G113" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="H118" s="16" t="s">
+      <c r="H113" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="I118" s="16" t="s">
+      <c r="I113" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="J118" s="28" t="s">
+      <c r="J113" s="28" t="s">
         <v>283</v>
       </c>
-      <c r="K118" s="16" t="s">
+      <c r="K113" s="16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A122" s="15"/>
-    </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A125" s="15"/>
-    </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A128" s="15"/>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="15"/>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="15"/>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="15"/>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="15"/>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="15"/>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="15"/>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" s="15"/>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" s="15"/>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" s="15"/>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="15"/>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" s="15"/>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" s="15"/>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" s="15"/>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A170" s="15"/>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A173" s="15"/>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176" s="15"/>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A179" s="15"/>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A182" s="15"/>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185" s="15"/>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A117" s="15"/>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A120" s="15"/>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A123" s="15"/>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A126" s="15"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="15"/>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="15"/>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="15"/>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="15"/>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="15"/>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="15"/>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="15"/>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="15"/>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="15"/>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="15"/>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="15"/>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="15"/>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="15"/>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="15"/>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="15"/>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="15"/>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="15"/>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
member edit and new
</commit_message>
<xml_diff>
--- a/Table descLAST.xlsx
+++ b/Table descLAST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altanbagana.n\source\repos\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4859DD-8062-49CF-8106-6F0EF175512F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0883BC0D-0585-4854-8710-BFDE055A7978}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1575" yWindow="1455" windowWidth="28170" windowHeight="12645" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1560" windowWidth="28170" windowHeight="12645" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -3354,8 +3354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="B121" sqref="B121"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="G117" sqref="G117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5019,7 +5019,7 @@
       <c r="L112" s="17"/>
       <c r="M112" s="17"/>
     </row>
-    <row r="113" spans="1:15" ht="78.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" ht="27.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A113" s="16" t="s">
         <v>3</v>
       </c>
@@ -5053,6 +5053,7 @@
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" s="15"/>
+      <c r="G117"/>
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119" s="15" t="s">

</xml_diff>

<commit_message>
big fix entityframework add ctype change states1 to state
</commit_message>
<xml_diff>
--- a/Table descLAST.xlsx
+++ b/Table descLAST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altanbagana.n\source\repos\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0883BC0D-0585-4854-8710-BFDE055A7978}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5EED81-6567-407B-BA59-918807850B82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1560" windowWidth="28170" windowHeight="12645" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -868,9 +868,6 @@
     <t>AssetBalances</t>
   </si>
   <si>
-    <t>1-долоо хоногийн өдрүүд</t>
-  </si>
-  <si>
     <t>1-Даваа, 2-Мягмар ... Өдрүүдийг ";" тэмдэгтээр тусгаарласан байна</t>
   </si>
   <si>
@@ -890,9 +887,6 @@
 5-Зах зээл үүсгэгч</t>
   </si>
   <si>
-    <t>Үнэт цаасны төрөл 1-үнэт цаас, 2-бонд</t>
-  </si>
-  <si>
     <t>гэрээний төрөл 1-спот, 2-форвард, 3-фьючерс, 4-опцион</t>
   </si>
   <si>
@@ -984,6 +978,12 @@
   </si>
   <si>
     <t>70xxh100</t>
+  </si>
+  <si>
+    <t>Үнэт цаасны төрөл 1-хувьцаа, 2-бонд</t>
+  </si>
+  <si>
+    <t>1-долоо хоногийн өдрүүд 2 сар</t>
   </si>
 </sst>
 </file>
@@ -3354,8 +3354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="G117" sqref="G117"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3421,7 +3421,7 @@
         <v>13</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G3" s="16" t="s">
         <v>15</v>
@@ -3429,10 +3429,10 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C4" s="28" t="s">
+        <v>318</v>
+      </c>
+      <c r="D4" s="28" t="s">
         <v>281</v>
-      </c>
-      <c r="D4" s="28" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -3520,19 +3520,19 @@
         <v>34</v>
       </c>
       <c r="F7" s="26" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G7" s="16" t="s">
         <v>36</v>
       </c>
       <c r="H7" s="29" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I7" s="16" t="s">
         <v>13</v>
       </c>
       <c r="J7" s="28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K7" s="16" t="s">
         <v>15</v>
@@ -3559,7 +3559,7 @@
         <v>44</v>
       </c>
       <c r="S7" s="26" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -3641,7 +3641,7 @@
         <v>72</v>
       </c>
       <c r="J11" s="28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K11" s="16" t="s">
         <v>15</v>
@@ -3719,7 +3719,7 @@
         <v>186</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>287</v>
+        <v>317</v>
       </c>
       <c r="D15" s="16" t="s">
         <v>66</v>
@@ -3749,7 +3749,7 @@
         <v>194</v>
       </c>
       <c r="N15" s="28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="O15" s="20" t="s">
         <v>15</v>
@@ -3820,7 +3820,7 @@
         <v>81</v>
       </c>
       <c r="G19" s="28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H19" s="16" t="s">
         <v>15</v>
@@ -3892,7 +3892,7 @@
         <v>201</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D23" s="16" t="s">
         <v>66</v>
@@ -3913,7 +3913,7 @@
         <v>205</v>
       </c>
       <c r="K23" s="28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L23" s="20" t="s">
         <v>15</v>
@@ -4009,7 +4009,7 @@
         <v>53</v>
       </c>
       <c r="K27" s="28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L27" s="17" t="s">
         <v>212</v>
@@ -4064,10 +4064,10 @@
         <v>159</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E31" s="26" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F31" s="16" t="s">
         <v>162</v>
@@ -4151,7 +4151,7 @@
         <v>174</v>
       </c>
       <c r="J35" s="28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K35" s="20" t="s">
         <v>15</v>
@@ -4226,7 +4226,7 @@
         <v>146</v>
       </c>
       <c r="I39" s="28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J39" s="16" t="s">
         <v>15</v>
@@ -4274,7 +4274,7 @@
         <v>224</v>
       </c>
       <c r="E43" s="28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F43" s="16" t="s">
         <v>212</v>
@@ -4316,7 +4316,7 @@
         <v>97</v>
       </c>
       <c r="D51" s="28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E51" s="16" t="s">
         <v>15</v>
@@ -4495,7 +4495,7 @@
         <v>3</v>
       </c>
       <c r="B67" s="26" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C67" s="16" t="s">
         <v>94</v>
@@ -4519,7 +4519,7 @@
         <v>80</v>
       </c>
       <c r="J67" s="28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K67" s="16" t="s">
         <v>15</v>
@@ -4574,7 +4574,7 @@
         <v>3</v>
       </c>
       <c r="B71" s="26" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C71" s="16" t="s">
         <v>112</v>
@@ -4598,7 +4598,7 @@
         <v>99</v>
       </c>
       <c r="J71" s="28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K71" s="16" t="s">
         <v>15</v>
@@ -4659,7 +4659,7 @@
         <v>13</v>
       </c>
       <c r="G75" s="28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H75" s="16" t="s">
         <v>15</v>
@@ -4818,46 +4818,46 @@
     </row>
     <row r="91" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="32" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B91" s="32"/>
     </row>
     <row r="92" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="32" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B92" s="32"/>
     </row>
     <row r="93" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="32" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B93" s="32"/>
     </row>
     <row r="94" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="32" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B94" s="32"/>
     </row>
     <row r="95" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="32" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B95" s="32"/>
     </row>
     <row r="96" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="32" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B96" s="32"/>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" s="15" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C98" s="16" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
@@ -4868,16 +4868,16 @@
         <v>88</v>
       </c>
       <c r="C99" s="16" t="s">
+        <v>299</v>
+      </c>
+      <c r="D99" s="16" t="s">
+        <v>300</v>
+      </c>
+      <c r="E99" s="16" t="s">
         <v>301</v>
       </c>
-      <c r="D99" s="16" t="s">
-        <v>302</v>
-      </c>
-      <c r="E99" s="16" t="s">
-        <v>303</v>
-      </c>
       <c r="F99" s="16" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G99" s="35" t="s">
         <v>9</v>
@@ -4891,7 +4891,7 @@
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" s="15" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G104"/>
     </row>
@@ -4900,10 +4900,10 @@
         <v>3</v>
       </c>
       <c r="B105" s="16" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C105" s="16" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D105" s="16" t="s">
         <v>9</v>
@@ -4927,7 +4927,7 @@
     </row>
     <row r="108" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="27" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B108" s="17" t="s">
         <v>85</v>
@@ -4936,7 +4936,7 @@
         <v>87</v>
       </c>
       <c r="D108" s="36" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E108" s="36" t="s">
         <v>89</v>
@@ -4951,10 +4951,10 @@
         <v>92</v>
       </c>
       <c r="I108" s="26" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="J108" s="26" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K108" s="17" t="s">
         <v>8</v>
@@ -4976,10 +4976,10 @@
     </row>
     <row r="111" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="15" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C111" s="16" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H111"/>
       <c r="I111"/>
@@ -5024,7 +5024,7 @@
         <v>3</v>
       </c>
       <c r="B113" s="26" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D113" s="16" t="s">
         <v>95</v>
@@ -5045,7 +5045,7 @@
         <v>80</v>
       </c>
       <c r="J113" s="28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K113" s="16" t="s">
         <v>15</v>
@@ -5105,10 +5105,10 @@
         <v>65</v>
       </c>
       <c r="N120" s="17" t="s">
+        <v>313</v>
+      </c>
+      <c r="O120" s="17" t="s">
         <v>315</v>
-      </c>
-      <c r="O120" s="17" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.25">
@@ -5116,7 +5116,7 @@
         <v>3</v>
       </c>
       <c r="B121" s="26" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C121" s="16" t="s">
         <v>66</v>
@@ -5140,13 +5140,13 @@
         <v>72</v>
       </c>
       <c r="J121" s="28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K121" s="16" t="s">
         <v>15</v>
       </c>
       <c r="O121" s="16" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
orderOk get dealType from BID
</commit_message>
<xml_diff>
--- a/Table descLAST.xlsx
+++ b/Table descLAST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altanbagana.n\source\repos\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18600AE-20B6-4290-A53E-2EBBB56EEECD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19239879-BFA5-4195-839A-820CD24E7C55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28920" yWindow="1560" windowWidth="28170" windowHeight="12645" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29430" yWindow="990" windowWidth="28170" windowHeight="12645" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="320">
   <si>
     <t>Boards</t>
   </si>
@@ -984,6 +984,9 @@
   </si>
   <si>
     <t>1-долоо хоногийн өдрүүд 2 сар</t>
+  </si>
+  <si>
+    <t>DEAL TYPE</t>
   </si>
 </sst>
 </file>
@@ -3352,10 +3355,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:S180"/>
+  <dimension ref="A5:S180"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3369,72 +3372,6 @@
     <col min="1026" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>282</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C4" s="28" t="s">
-        <v>318</v>
-      </c>
-      <c r="D4" s="28" t="s">
-        <v>281</v>
-      </c>
-    </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>16</v>
@@ -4446,85 +4383,6 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="B65" s="15"/>
-      <c r="C65" s="15" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B66" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="C66" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="D66" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="E66" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="F66" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="G66" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="H66" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="I66" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="J66" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="K66" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B67" s="26" t="s">
-        <v>290</v>
-      </c>
-      <c r="C67" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="D67" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="E67" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="F67" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="G67" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="H67" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="I67" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="J67" s="28" t="s">
-        <v>282</v>
-      </c>
-      <c r="K67" s="16" t="s">
-        <v>15</v>
-      </c>
-    </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="15" t="s">
         <v>100</v>
@@ -5152,25 +5010,177 @@
     <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A123" s="15"/>
     </row>
+    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J124" s="37"/>
+    </row>
     <row r="126" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A126" s="15"/>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="15"/>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A127" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B127" s="15"/>
+      <c r="C127" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G127" s="17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A128" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B128" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C128" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D128" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E128" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F128" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G128" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H128" s="37" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A129" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B129" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C129" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D129" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E129" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F129" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="G129" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H129" s="37"/>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C130" s="28" t="s">
+        <v>318</v>
+      </c>
+      <c r="D130" s="28" t="s">
+        <v>281</v>
+      </c>
+      <c r="H130" s="37"/>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" s="15"/>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="15"/>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A134" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B134" s="15"/>
+      <c r="C134" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="L134" s="37" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A135" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B135" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C135" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="D135" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E135" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="F135" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="G135" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="H135" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="I135" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="J135" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="K135" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="L135" s="37"/>
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A136" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B136" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="C136" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D136" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="E136" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="F136" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="G136" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="H136" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="I136" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="J136" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="K136" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="L136" s="37"/>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138" s="15"/>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141" s="15"/>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A144" s="15"/>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>